<commit_message>
new changes by client
</commit_message>
<xml_diff>
--- a/public/sample.xlsx
+++ b/public/sample.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\smart_campus\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEE28BA0-AA38-471A-B7D4-34008BF2F47D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1914706F-7DA5-477F-A7EC-ED7A49901847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{6D156CF1-58B3-4A6B-A220-7B0D5E6B5C9D}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">Sl. No </t>
   </si>
@@ -81,6 +81,21 @@
   </si>
   <si>
     <t>Birth Date(dd/mm/yyyy)</t>
+  </si>
+  <si>
+    <t>Previous College Address</t>
+  </si>
+  <si>
+    <t>Previous College Contact</t>
+  </si>
+  <si>
+    <t>Previous College contact Person</t>
+  </si>
+  <si>
+    <t>Previous College contact Person Email</t>
+  </si>
+  <si>
+    <t>Previous College contact Person password</t>
   </si>
 </sst>
 </file>
@@ -477,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98D1DB57-7FC3-498D-B16A-6AC2E2717F17}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,20 +503,25 @@
     <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="39.28515625" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="24.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="23.28515625" style="2" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="2"/>
-    <col min="10" max="10" width="11.85546875" style="2" customWidth="1"/>
-    <col min="11" max="12" width="14" style="2" customWidth="1"/>
-    <col min="13" max="13" width="22.5703125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="17.85546875" style="2" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="2"/>
+    <col min="4" max="4" width="19.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="25" style="2" customWidth="1"/>
+    <col min="9" max="9" width="26.85546875" style="2" customWidth="1"/>
+    <col min="10" max="11" width="24.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="2"/>
+    <col min="16" max="16" width="11.85546875" style="2" customWidth="1"/>
+    <col min="17" max="18" width="14" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.5703125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,48 +535,63 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="4"/>
-    </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="4"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -564,17 +599,23 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
       <c r="G2" s="5"/>
-      <c r="H2" s="6"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
+      <c r="N2" s="6"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -582,17 +623,23 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
-      <c r="H3" s="6"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
+      <c r="N3" s="6"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
+      <c r="V3" s="5"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -600,17 +647,23 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
+      <c r="N4" s="6"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -627,8 +680,14 @@
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -645,8 +704,14 @@
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="5"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -663,8 +728,14 @@
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="5"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -681,8 +752,14 @@
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -699,8 +776,14 @@
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -717,8 +800,14 @@
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="5"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -735,8 +824,14 @@
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q11" s="5"/>
+      <c r="R11" s="5"/>
+      <c r="S11" s="5"/>
+      <c r="T11" s="5"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="5"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -753,8 +848,14 @@
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q12" s="5"/>
+      <c r="R12" s="5"/>
+      <c r="S12" s="5"/>
+      <c r="T12" s="5"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="5"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -771,8 +872,14 @@
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q13" s="5"/>
+      <c r="R13" s="5"/>
+      <c r="S13" s="5"/>
+      <c r="T13" s="5"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="5"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -789,8 +896,14 @@
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q14" s="5"/>
+      <c r="R14" s="5"/>
+      <c r="S14" s="5"/>
+      <c r="T14" s="5"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="5"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -807,8 +920,14 @@
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="5"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
@@ -825,8 +944,14 @@
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q16" s="5"/>
+      <c r="R16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="5"/>
@@ -843,8 +968,14 @@
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+      <c r="S17" s="5"/>
+      <c r="T17" s="5"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="5"/>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
@@ -861,8 +992,14 @@
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+      <c r="S18" s="5"/>
+      <c r="T18" s="5"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="5"/>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -879,8 +1016,14 @@
       <c r="N19" s="5"/>
       <c r="O19" s="5"/>
       <c r="P19" s="5"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+      <c r="S19" s="5"/>
+      <c r="T19" s="5"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="5"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
       <c r="C20" s="5"/>
@@ -897,8 +1040,14 @@
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+      <c r="S20" s="5"/>
+      <c r="T20" s="5"/>
+      <c r="U20" s="5"/>
+      <c r="V20" s="5"/>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -915,8 +1064,14 @@
       <c r="N21" s="5"/>
       <c r="O21" s="5"/>
       <c r="P21" s="5"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+      <c r="S21" s="5"/>
+      <c r="T21" s="5"/>
+      <c r="U21" s="5"/>
+      <c r="V21" s="5"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
@@ -933,6 +1088,12 @@
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+      <c r="S22" s="5"/>
+      <c r="T22" s="5"/>
+      <c r="U22" s="5"/>
+      <c r="V22" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>